<commit_message>
feat: add excel/csv import and export for rules
- Implemented `ImportExportService` for parsing/generating Excel and CSV.
- Added `/api/admin/import/preview` and `/api/admin/import/rules` endpoints.
- Updated `storage.importUrlRules` to support upsert (update existing, insert new).
- Refactored Admin UI to split Standard (Excel/CSV) and Advanced (JSON) imports.
- Added environment variable `IMPORT_PREVIEW_LIMIT` (default 1000).
- Updated documentation and sample files.
- Ensured backward compatibility for JSON import.
</commit_message>
<xml_diff>
--- a/sample-rules-import.xlsx
+++ b/sample-rules-import.xlsx
@@ -397,74 +397,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ID</v>
+        <v>Matcher</v>
       </c>
       <c r="B1" t="str">
-        <v>Matcher</v>
-      </c>
-      <c r="C1" t="str">
         <v>Target URL</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Type</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Info</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Auto Redirect</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>uuid-placeholder-1</v>
+        <v>/old-page</v>
       </c>
       <c r="B2" t="str">
-        <v>/old-page</v>
-      </c>
-      <c r="C2" t="str">
         <v>https://example.com/new-page</v>
-      </c>
-      <c r="D2" t="str">
-        <v>partial</v>
-      </c>
-      <c r="E2" t="str">
-        <v>Simple partial redirect</v>
-      </c>
-      <c r="F2" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>uuid-placeholder-2</v>
+        <v>/legacy-section</v>
       </c>
       <c r="B3" t="str">
-        <v>/legacy-section</v>
-      </c>
-      <c r="C3" t="str">
         <v>https://example.com/modern-section</v>
-      </c>
-      <c r="D3" t="str">
-        <v>wildcard</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Wildcard redirect with auto-redirect enabled</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Optimize Importer/Exporter and Fix Crashes
- Replaced `xlsx` with `@e965/xlsx` for better compatibility.
- Fixed server crash in Excel export error handling.
- Fixed CSV export to return proper CSV format instead of JSON.
- Enhanced Import Preview UI with client-side pagination (default 50, load more).
- Updated sample files generation to include all required columns.
- Separated Settings Import/Export from Rules/Stats in Admin UI.
- Improved Import button UI and descriptions.
</commit_message>
<xml_diff>
--- a/sample-rules-import.xlsx
+++ b/sample-rules-import.xlsx
@@ -397,38 +397,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>ID</v>
+      </c>
+      <c r="B1" t="str">
         <v>Matcher</v>
       </c>
-      <c r="B1" t="str">
+      <c r="C1" t="str">
         <v>Target URL</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Type</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Info</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Auto Redirect</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
+        <v/>
+      </c>
+      <c r="B2" t="str">
         <v>/old-page</v>
       </c>
-      <c r="B2" t="str">
+      <c r="C2" t="str">
         <v>https://example.com/new-page</v>
+      </c>
+      <c r="D2" t="str">
+        <v>partial</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Sample Redirect</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
+        <v/>
+      </c>
+      <c r="B3" t="str">
         <v>/legacy-section</v>
       </c>
-      <c r="B3" t="str">
+      <c r="C3" t="str">
         <v>https://example.com/modern-section</v>
+      </c>
+      <c r="D3" t="str">
+        <v>wildcard</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Legacy Section Redirect</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs: fix misleading sample import rules
Updates `scripts/generate-samples.ts` to swap the redirect types of the sample rules:
- `/old-page` is now a `wildcard` (exact) redirect.
- `/legacy-section` is now a `partial` (prefix) redirect.
This addresses user confusion regarding invalid or nonsensical rule types in the provided sample files.
Regenerated `sample-rules-import.csv`, `sample-rules-import.xlsx`, and `sample-rules-import.json`.
</commit_message>
<xml_diff>
--- a/sample-rules-import.xlsx
+++ b/sample-rules-import.xlsx
@@ -433,10 +433,10 @@
         <v>https://example.com/new-page</v>
       </c>
       <c r="D2" t="str">
-        <v>partial</v>
+        <v>wildcard</v>
       </c>
       <c r="E2" t="str">
-        <v>Sample Redirect</v>
+        <v>Exact Page Redirect</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -453,10 +453,10 @@
         <v>https://example.com/modern-section</v>
       </c>
       <c r="D3" t="str">
-        <v>wildcard</v>
+        <v>partial</v>
       </c>
       <c r="E3" t="str">
-        <v>Legacy Section Redirect</v>
+        <v>Section/Folder Redirect</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
docs: fix misleading sample import rules and add missing columns
Updates `scripts/generate-samples.ts` to:
1. Swap the redirect types of the sample rules:
   - `/old-page` is now a `wildcard` (exact) redirect.
   - `/legacy-section` is now a `partial` (prefix) redirect with a relative target path (`/modern-section`).
2. Add missing columns 'Discard Query Params' and 'Keep Query Params' to CSV and Excel samples.
3. Add corresponding `discardQueryParams` and `forwardQueryParams` fields to the JSON sample.

This addresses user confusion regarding invalid rule types and ensures the samples reflect all available configuration options.
Regenerated `sample-rules-import.csv`, `sample-rules-import.xlsx`, and `sample-rules-import.json`.
</commit_message>
<xml_diff>
--- a/sample-rules-import.xlsx
+++ b/sample-rules-import.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -421,6 +421,12 @@
       <c r="F1" t="str">
         <v>Auto Redirect</v>
       </c>
+      <c r="G1" t="str">
+        <v>Discard Query Params</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Keep Query Params</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -441,6 +447,12 @@
       <c r="F2" t="b">
         <v>0</v>
       </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -461,10 +473,16 @@
       <c r="F3" t="b">
         <v>1</v>
       </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>